<commit_message>
Clean and comment e2eOrder, visit, login and register test scripts for recording test videoes
</commit_message>
<xml_diff>
--- a/cypress/fixtures/testCaseCriteria/testCaseCriteria_e2eOrder.xlsx
+++ b/cypress/fixtures/testCaseCriteria/testCaseCriteria_e2eOrder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\awika-portfolio\automationexercise\cypress\fixtures\testCaseCriteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6912C1-DFFC-448C-9DEB-A52F36F4E373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6D9250-A55F-483F-867A-56AB3B68DCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6090" yWindow="-14865" windowWidth="28455" windowHeight="11880" tabRatio="553" activeTab="1" xr2:uid="{63A55816-40FB-44DD-8B96-272E0273596B}"/>
+    <workbookView xWindow="11085" yWindow="-14865" windowWidth="23460" windowHeight="11880" tabRatio="553" activeTab="1" xr2:uid="{63A55816-40FB-44DD-8B96-272E0273596B}"/>
   </bookViews>
   <sheets>
     <sheet name="column_ref" sheetId="20" r:id="rId1"/>
@@ -770,7 +770,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1111,7 +1111,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1847,7 +1847,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>